<commit_message>
Updated the farm layout to match what's seen in-game
</commit_message>
<xml_diff>
--- a/structure/Turtle Farm - Crops.xlsx
+++ b/structure/Turtle Farm - Crops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\C\Projetos\Heartbound Save Editor\structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2594F84F-5B8F-41EE-BCF4-AB4AB095DFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2322E6-7D6E-4DE3-8B58-21A38F334956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,10 +492,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,7 +789,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -811,8 +810,8 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="2" t="s">
-        <v>45</v>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -832,10 +831,10 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>44</v>
@@ -846,10 +845,10 @@
         <v>49</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -858,25 +857,25 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -884,36 +883,36 @@
         <v>50</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>34</v>
@@ -922,7 +921,7 @@
         <v>39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -930,106 +929,106 @@
         <v>51</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1052,86 +1051,86 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1148,140 +1147,140 @@
         <v>81</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="M11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="O11" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="H12" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="L12" s="1" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="I13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1292,16 +1291,16 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1318,16 +1317,16 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>

</xml_diff>